<commit_message>
yönetim sayfasına arama kutucuğu ve tür listesi eklendi.
türler ve kullanıcı isteğine göre db'den çekildi.
</commit_message>
<xml_diff>
--- a/database/veri.xlsx
+++ b/database/veri.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bthn0\Desktop\NetflixVeritabaniProjesi\database\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\NetflixVeritabaniProjesi\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FA749B2-796D-4E22-AD91-B15C2E88505B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3765F37-AD0B-4CDE-9DDF-C4BB9984EA6B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="2025" yWindow="1365" windowWidth="21600" windowHeight="11325" xr2:uid="{A0B0D475-3B95-4965-B38F-CC433C426B96}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="19956" windowHeight="8892" xr2:uid="{A0B0D475-3B95-4965-B38F-CC433C426B96}"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
@@ -180,102 +180,15 @@
     <t>Cocuk ve Aile</t>
   </si>
   <si>
-    <t>Alaca Karanlik</t>
-  </si>
-  <si>
     <t>Jurassic Park</t>
   </si>
   <si>
-    <t>Bizi Hatirla</t>
-  </si>
-  <si>
-    <t>Trol Avcilari: Arcadia Hikayeleri</t>
-  </si>
-  <si>
-    <t>Sunger Bob</t>
-  </si>
-  <si>
-    <t>Buyuk Tasarimlar</t>
-  </si>
-  <si>
-    <t>Beni Boyle Sev</t>
-  </si>
-  <si>
-    <t>Recep Ivedik 6</t>
-  </si>
-  <si>
-    <t>Yuzuklerin Efendisi Iki Kule</t>
-  </si>
-  <si>
-    <t>Kuslarla Dans</t>
-  </si>
-  <si>
-    <t>Mercan Pesinde</t>
-  </si>
-  <si>
-    <t>Marsta Kesif</t>
-  </si>
-  <si>
-    <t>Kardesim Benim</t>
-  </si>
-  <si>
-    <t>Masa ve Koca Ayi</t>
-  </si>
-  <si>
-    <t>Kung Fu Panda Muhtesem Sirlar</t>
-  </si>
-  <si>
-    <t>Dunyanin En Sira Disi Evleri</t>
-  </si>
-  <si>
-    <t>Siradisi Kulubeler</t>
-  </si>
-  <si>
-    <t>Baslangic</t>
-  </si>
-  <si>
-    <t>Kuscular</t>
-  </si>
-  <si>
-    <t>Yercekimi</t>
-  </si>
-  <si>
-    <t>Kara Sovalye</t>
-  </si>
-  <si>
-    <t>Sirinler</t>
-  </si>
-  <si>
-    <t>Da Vinci Sifresi</t>
-  </si>
-  <si>
-    <t>Orumcek Adam</t>
-  </si>
-  <si>
-    <t>Transformers Kayip Cag</t>
-  </si>
-  <si>
-    <t>Ninja Kaplumbagalar</t>
-  </si>
-  <si>
-    <t>Dirilis Ertugrul</t>
-  </si>
-  <si>
     <t>PK</t>
   </si>
   <si>
-    <t>Yuzuklerin Efendisi Kralin Donusu</t>
-  </si>
-  <si>
-    <t>Harry Potter Olum Yadigarlari</t>
-  </si>
-  <si>
     <t>How I Met Your Mother</t>
   </si>
   <si>
-    <t>Patron Bebek Yine Is Basinda</t>
-  </si>
-  <si>
     <t>Aksiyon ve Macera,Bilim Kurgu ve Fantastik Yapimlar</t>
   </si>
   <si>
@@ -330,9 +243,6 @@
     <t>Aydaki Son Adam</t>
   </si>
   <si>
-    <t>Charlienin Cikolata Fabrikasi</t>
-  </si>
-  <si>
     <t>Marwel Iron Fist</t>
   </si>
   <si>
@@ -349,6 +259,96 @@
   </si>
   <si>
     <t>s</t>
+  </si>
+  <si>
+    <t>Recep İvedik 6</t>
+  </si>
+  <si>
+    <t>Alaca Karanlık</t>
+  </si>
+  <si>
+    <t>Yüzüklerin Efendisi İki Kule</t>
+  </si>
+  <si>
+    <t>Kara Şövalye</t>
+  </si>
+  <si>
+    <t>Transformers Kayıp Çağ</t>
+  </si>
+  <si>
+    <t>Başlangıç</t>
+  </si>
+  <si>
+    <t>Ninja Kaplumbağalar</t>
+  </si>
+  <si>
+    <t>Kuşlarla Dans</t>
+  </si>
+  <si>
+    <t>Mercan Peşinde</t>
+  </si>
+  <si>
+    <t>Örümcek Adam</t>
+  </si>
+  <si>
+    <t>Kuşçular</t>
+  </si>
+  <si>
+    <t>Marsta Keşif</t>
+  </si>
+  <si>
+    <t>Şirinler</t>
+  </si>
+  <si>
+    <t>Bizi Hatırla</t>
+  </si>
+  <si>
+    <t>Kardeşim Benim</t>
+  </si>
+  <si>
+    <t>Yerçekimi</t>
+  </si>
+  <si>
+    <t>Da Vinci Şifresi</t>
+  </si>
+  <si>
+    <t>Diriliş Ertuğrul</t>
+  </si>
+  <si>
+    <t>Trol Avcıları: Arcadia Hikayeleri</t>
+  </si>
+  <si>
+    <t>Beni Böyle Sev</t>
+  </si>
+  <si>
+    <t>Maşa ve Koca Ayı</t>
+  </si>
+  <si>
+    <t>Sünger Bob</t>
+  </si>
+  <si>
+    <t>Kung Fu Panda Muhteşem Sırlar</t>
+  </si>
+  <si>
+    <t>Dünyanın En Sıra Dışı Evleri</t>
+  </si>
+  <si>
+    <t>Büyük Tasarımlar</t>
+  </si>
+  <si>
+    <t>Sıradışı Kulübeler</t>
+  </si>
+  <si>
+    <t>Charlienin Çikolata Fabrikası</t>
+  </si>
+  <si>
+    <t>Harry Potter Ölüm Yadigarları</t>
+  </si>
+  <si>
+    <t>Yüzüklerin Efendisi Kralın Dönüşü</t>
+  </si>
+  <si>
+    <t>Patron Bebek Yine İş Başında</t>
   </si>
 </sst>
 </file>
@@ -385,9 +385,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -704,22 +705,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8717F3CD-EC94-4834-B4A7-0917B9E8CEB1}">
   <dimension ref="A1:I75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="I74" sqref="I74"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="A58" sqref="A58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="34.7109375" customWidth="1"/>
+    <col min="1" max="1" width="34.6640625" customWidth="1"/>
     <col min="2" max="2" width="68" customWidth="1"/>
-    <col min="4" max="4" width="6.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="7.140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="8.85546875" style="1"/>
+    <col min="4" max="4" width="6.6640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="7.109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>56</v>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>76</v>
       </c>
       <c r="B1" t="s">
         <v>5</v>
@@ -737,12 +738,12 @@
         <v>120</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>97</v>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>68</v>
       </c>
       <c r="B2" t="s">
-        <v>81</v>
+        <v>52</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
@@ -757,12 +758,12 @@
         <v>160</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>49</v>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>77</v>
       </c>
       <c r="B3" t="s">
-        <v>82</v>
+        <v>53</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
@@ -777,12 +778,12 @@
         <v>180</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>57</v>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>78</v>
       </c>
       <c r="B4" t="s">
-        <v>81</v>
+        <v>52</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
@@ -797,12 +798,12 @@
         <v>90</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>81</v>
+        <v>52</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
@@ -817,12 +818,12 @@
         <v>130</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>69</v>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>79</v>
       </c>
       <c r="B6" t="s">
-        <v>81</v>
+        <v>52</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>
@@ -837,8 +838,8 @@
         <v>150</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B7" t="s">
@@ -857,12 +858,12 @@
         <v>145</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>77</v>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>104</v>
       </c>
       <c r="B8" t="s">
-        <v>81</v>
+        <v>52</v>
       </c>
       <c r="C8" t="s">
         <v>6</v>
@@ -877,9 +878,9 @@
         <v>88</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>73</v>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>80</v>
       </c>
       <c r="B9" t="s">
         <v>5</v>
@@ -897,9 +898,9 @@
         <v>96</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>66</v>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>81</v>
       </c>
       <c r="B10" t="s">
         <v>5</v>
@@ -917,12 +918,12 @@
         <v>95</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>96</v>
+        <v>67</v>
       </c>
       <c r="C11" t="s">
         <v>6</v>
@@ -937,12 +938,12 @@
         <v>120</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>78</v>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>103</v>
       </c>
       <c r="B12" t="s">
-        <v>83</v>
+        <v>54</v>
       </c>
       <c r="C12" t="s">
         <v>6</v>
@@ -957,8 +958,8 @@
         <v>160</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B13" t="s">
@@ -977,12 +978,12 @@
         <v>180</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B14" t="s">
-        <v>101</v>
+        <v>71</v>
       </c>
       <c r="C14" t="s">
         <v>6</v>
@@ -997,12 +998,12 @@
         <v>90</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>74</v>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>82</v>
       </c>
       <c r="B15" t="s">
-        <v>81</v>
+        <v>52</v>
       </c>
       <c r="C15" t="s">
         <v>6</v>
@@ -1017,9 +1018,9 @@
         <v>130</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>58</v>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>83</v>
       </c>
       <c r="B16" t="s">
         <v>7</v>
@@ -1037,8 +1038,8 @@
         <v>150</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B17" t="s">
@@ -1057,9 +1058,9 @@
         <v>145</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>59</v>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>84</v>
       </c>
       <c r="B18" t="s">
         <v>7</v>
@@ -1077,8 +1078,8 @@
         <v>88</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B19" t="s">
@@ -1097,9 +1098,9 @@
         <v>96</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>98</v>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>69</v>
       </c>
       <c r="B20" t="s">
         <v>7</v>
@@ -1117,8 +1118,8 @@
         <v>95</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B21" t="s">
@@ -1137,8 +1138,8 @@
         <v>120</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B22" t="s">
@@ -1157,8 +1158,8 @@
         <v>160</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B23" t="s">
@@ -1177,12 +1178,12 @@
         <v>180</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B24" t="s">
-        <v>84</v>
+        <v>55</v>
       </c>
       <c r="C24" t="s">
         <v>6</v>
@@ -1197,12 +1198,12 @@
         <v>90</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>76</v>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>50</v>
       </c>
       <c r="B25" t="s">
-        <v>85</v>
+        <v>56</v>
       </c>
       <c r="C25" t="s">
         <v>6</v>
@@ -1217,12 +1218,12 @@
         <v>130</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>72</v>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>85</v>
       </c>
       <c r="B26" t="s">
-        <v>81</v>
+        <v>52</v>
       </c>
       <c r="C26" t="s">
         <v>6</v>
@@ -1237,12 +1238,12 @@
         <v>150</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>50</v>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
+        <v>49</v>
       </c>
       <c r="B27" t="s">
-        <v>103</v>
+        <v>73</v>
       </c>
       <c r="C27" t="s">
         <v>6</v>
@@ -1257,12 +1258,12 @@
         <v>145</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B28" t="s">
-        <v>104</v>
+        <v>74</v>
       </c>
       <c r="C28" t="s">
         <v>6</v>
@@ -1277,12 +1278,12 @@
         <v>88</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B29" t="s">
-        <v>86</v>
+        <v>57</v>
       </c>
       <c r="C29" t="s">
         <v>6</v>
@@ -1297,12 +1298,12 @@
         <v>96</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B30" t="s">
-        <v>86</v>
+        <v>57</v>
       </c>
       <c r="C30" t="s">
         <v>6</v>
@@ -1317,12 +1318,12 @@
         <v>95</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>67</v>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
+        <v>86</v>
       </c>
       <c r="B31" t="s">
-        <v>86</v>
+        <v>57</v>
       </c>
       <c r="C31" t="s">
         <v>6</v>
@@ -1337,12 +1338,12 @@
         <v>120</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>60</v>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
+        <v>87</v>
       </c>
       <c r="B32" t="s">
-        <v>86</v>
+        <v>57</v>
       </c>
       <c r="C32" t="s">
         <v>6</v>
@@ -1357,12 +1358,12 @@
         <v>160</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B33" t="s">
-        <v>86</v>
+        <v>57</v>
       </c>
       <c r="C33" t="s">
         <v>6</v>
@@ -1377,12 +1378,12 @@
         <v>180</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B34" t="s">
-        <v>86</v>
+        <v>57</v>
       </c>
       <c r="C34" t="s">
         <v>6</v>
@@ -1397,8 +1398,8 @@
         <v>90</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B35" t="s">
@@ -1417,12 +1418,12 @@
         <v>130</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>70</v>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" s="2" t="s">
+        <v>88</v>
       </c>
       <c r="B36" t="s">
-        <v>87</v>
+        <v>58</v>
       </c>
       <c r="C36" t="s">
         <v>6</v>
@@ -1437,12 +1438,12 @@
         <v>150</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>99</v>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" s="2" t="s">
+        <v>102</v>
       </c>
       <c r="B37" t="s">
-        <v>87</v>
+        <v>58</v>
       </c>
       <c r="C37" t="s">
         <v>6</v>
@@ -1457,8 +1458,8 @@
         <v>145</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B38" t="s">
@@ -1477,8 +1478,8 @@
         <v>88</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B39" t="s">
@@ -1497,12 +1498,12 @@
         <v>96</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B40" t="s">
-        <v>88</v>
+        <v>59</v>
       </c>
       <c r="C40" t="s">
         <v>6</v>
@@ -1517,8 +1518,8 @@
         <v>95</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B41" t="s">
@@ -1537,12 +1538,12 @@
         <v>120</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B42" t="s">
-        <v>87</v>
+        <v>58</v>
       </c>
       <c r="C42" t="s">
         <v>6</v>
@@ -1557,12 +1558,12 @@
         <v>160</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B43" t="s">
-        <v>87</v>
+        <v>58</v>
       </c>
       <c r="C43" t="s">
         <v>6</v>
@@ -1577,9 +1578,9 @@
         <v>180</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>51</v>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44" s="2" t="s">
+        <v>89</v>
       </c>
       <c r="B44" t="s">
         <v>25</v>
@@ -1597,12 +1598,12 @@
         <v>90</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A45" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B45" t="s">
-        <v>92</v>
+        <v>63</v>
       </c>
       <c r="C45" t="s">
         <v>6</v>
@@ -1617,12 +1618,12 @@
         <v>130</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>61</v>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A46" s="2" t="s">
+        <v>90</v>
       </c>
       <c r="B46" t="s">
-        <v>89</v>
+        <v>60</v>
       </c>
       <c r="C46" t="s">
         <v>6</v>
@@ -1637,8 +1638,8 @@
         <v>150</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A47" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B47" t="s">
@@ -1657,12 +1658,12 @@
         <v>145</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>68</v>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A48" s="2" t="s">
+        <v>91</v>
       </c>
       <c r="B48" t="s">
-        <v>90</v>
+        <v>61</v>
       </c>
       <c r="C48" t="s">
         <v>6</v>
@@ -1677,8 +1678,8 @@
         <v>88</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A49" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B49" t="s">
@@ -1697,9 +1698,9 @@
         <v>96</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>71</v>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A50" s="2" t="s">
+        <v>92</v>
       </c>
       <c r="B50" t="s">
         <v>29</v>
@@ -1717,9 +1718,9 @@
         <v>95</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>100</v>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A51" s="2" t="s">
+        <v>70</v>
       </c>
       <c r="B51" t="s">
         <v>5</v>
@@ -1737,12 +1738,12 @@
         <v>60</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A52" s="2" t="s">
         <v>31</v>
       </c>
       <c r="B52" t="s">
-        <v>88</v>
+        <v>59</v>
       </c>
       <c r="C52" t="s">
         <v>30</v>
@@ -1757,9 +1758,9 @@
         <v>55</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>75</v>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A53" s="2" t="s">
+        <v>93</v>
       </c>
       <c r="B53" t="s">
         <v>5</v>
@@ -1777,12 +1778,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>52</v>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A54" s="2" t="s">
+        <v>94</v>
       </c>
       <c r="B54" t="s">
-        <v>88</v>
+        <v>59</v>
       </c>
       <c r="C54" t="s">
         <v>30</v>
@@ -1797,9 +1798,9 @@
         <v>45</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>79</v>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A55" s="2" t="s">
+        <v>51</v>
       </c>
       <c r="B55" t="s">
         <v>33</v>
@@ -1817,8 +1818,8 @@
         <v>48</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A56" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B56" t="s">
@@ -1837,12 +1838,12 @@
         <v>66</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>55</v>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A57" s="2" t="s">
+        <v>95</v>
       </c>
       <c r="B57" t="s">
-        <v>92</v>
+        <v>63</v>
       </c>
       <c r="C57" t="s">
         <v>30</v>
@@ -1857,12 +1858,12 @@
         <v>70</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>80</v>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A58" s="2" t="s">
+        <v>105</v>
       </c>
       <c r="B58" t="s">
-        <v>87</v>
+        <v>58</v>
       </c>
       <c r="C58" t="s">
         <v>30</v>
@@ -1877,12 +1878,12 @@
         <v>54</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A59" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B59" t="s">
-        <v>82</v>
+        <v>53</v>
       </c>
       <c r="C59" t="s">
         <v>30</v>
@@ -1897,9 +1898,9 @@
         <v>60</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>62</v>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A60" s="2" t="s">
+        <v>96</v>
       </c>
       <c r="B60" t="s">
         <v>48</v>
@@ -1917,12 +1918,12 @@
         <v>55</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>53</v>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A61" s="2" t="s">
+        <v>97</v>
       </c>
       <c r="B61" t="s">
-        <v>87</v>
+        <v>58</v>
       </c>
       <c r="C61" t="s">
         <v>30</v>
@@ -1937,12 +1938,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A62" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B62" t="s">
-        <v>91</v>
+        <v>62</v>
       </c>
       <c r="C62" t="s">
         <v>30</v>
@@ -1957,12 +1958,12 @@
         <v>45</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A63" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B63" t="s">
-        <v>102</v>
+        <v>72</v>
       </c>
       <c r="C63" t="s">
         <v>30</v>
@@ -1977,12 +1978,12 @@
         <v>48</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A64" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B64" t="s">
-        <v>87</v>
+        <v>58</v>
       </c>
       <c r="C64" t="s">
         <v>30</v>
@@ -1997,8 +1998,8 @@
         <v>66</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A65" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B65" t="s">
@@ -2017,12 +2018,12 @@
         <v>70</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A66" s="2" t="s">
         <v>45</v>
       </c>
       <c r="B66" t="s">
-        <v>93</v>
+        <v>64</v>
       </c>
       <c r="C66" t="s">
         <v>30</v>
@@ -2037,12 +2038,12 @@
         <v>54</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A67" s="2" t="s">
         <v>46</v>
       </c>
       <c r="B67" t="s">
-        <v>94</v>
+        <v>65</v>
       </c>
       <c r="C67" t="s">
         <v>30</v>
@@ -2057,9 +2058,9 @@
         <v>60</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>63</v>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A68" s="2" t="s">
+        <v>98</v>
       </c>
       <c r="B68" t="s">
         <v>5</v>
@@ -2077,12 +2078,12 @@
         <v>55</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A69" s="2" t="s">
         <v>39</v>
       </c>
       <c r="B69" t="s">
-        <v>95</v>
+        <v>66</v>
       </c>
       <c r="C69" t="s">
         <v>30</v>
@@ -2097,9 +2098,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>64</v>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A70" s="2" t="s">
+        <v>99</v>
       </c>
       <c r="B70" t="s">
         <v>40</v>
@@ -2117,8 +2118,8 @@
         <v>45</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A71" s="2" t="s">
         <v>41</v>
       </c>
       <c r="B71" t="s">
@@ -2137,9 +2138,9 @@
         <v>48</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>54</v>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A72" s="2" t="s">
+        <v>100</v>
       </c>
       <c r="B72" t="s">
         <v>40</v>
@@ -2157,8 +2158,8 @@
         <v>66</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A73" s="2" t="s">
         <v>42</v>
       </c>
       <c r="B73" t="s">
@@ -2177,8 +2178,8 @@
         <v>70</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A74" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B74" t="s">
@@ -2197,12 +2198,12 @@
         <v>54</v>
       </c>
       <c r="I74" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>65</v>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A75" s="2" t="s">
+        <v>101</v>
       </c>
       <c r="B75" t="s">
         <v>40</v>

</xml_diff>